<commit_message>
implement scenarios for alternative feedstocks, products, and fermentation assumptions
</commit_message>
<xml_diff>
--- a/biorefineries/HP/analyses/full/parameter_distributions/HP_salt_product/parameter-distributions_glucose_HP-salt_10L.xlsx
+++ b/biorefineries/HP/analyses/full/parameter_distributions/HP_salt_product/parameter-distributions_glucose_HP-salt_10L.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\repository_clones\Bioindustrial-Park\biorefineries\HP\analyses\full\parameter_distributions\HP_salt_product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1C08F4-C246-4D77-A199-572B66944A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1244B4F1-20E2-4CC2-9E2E-281E431D4AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -686,7 +686,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -823,20 +823,19 @@
         <v>9</v>
       </c>
       <c r="E4" s="4">
-        <v>0.83730000000000004</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G4" s="4">
-        <v>0.79369999999999996</v>
+        <v>0.23</v>
       </c>
       <c r="H4" s="4">
-        <f>E4</f>
-        <v>0.83730000000000004</v>
+        <v>0.27</v>
       </c>
       <c r="I4" s="4">
-        <v>0.87080000000000002</v>
+        <v>0.34</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -844,7 +843,7 @@
       </c>
       <c r="Q4" s="5">
         <f t="shared" ref="Q4" si="0">IF(E4=H4, 1, IF(F4=$F$2, 1, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">

</xml_diff>